<commit_message>
fully workng code with updated visuals and full comments
</commit_message>
<xml_diff>
--- a/assets/StudyHistory.xlsx
+++ b/assets/StudyHistory.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,11 +454,6 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -470,57 +461,54 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DMP</t>
+          <t>test subject</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DMP Assignment 1</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>45817</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>test summary</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>16/06/2025</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>10</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>DMP</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>DMP Assignment 1</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>45817</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>16/06/2025</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>lhjjkhg</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>hhhh</t>
-        </is>
-      </c>
+      <c r="A4" t="n">
+        <v>25</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>15/06/2025</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>3</v>
+          <t>16/06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>16/06/2025</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final commit and removal of notes for assignment submission
</commit_message>
<xml_diff>
--- a/assets/StudyHistory.xlsx
+++ b/assets/StudyHistory.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,8 +479,16 @@
       <c r="A3" t="n">
         <v>4</v>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>tesing 2 subject</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>summary test 2</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>16/06/2025</t>
@@ -491,8 +499,16 @@
       <c r="A4" t="n">
         <v>25</v>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>subject test 3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>summary test 3</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>16/06/2025</t>
@@ -503,11 +519,59 @@
       <c r="A5" t="n">
         <v>5</v>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4th subject test</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5th summary test</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>16/06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>25</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>test 1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>syummary test</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>dhskfh</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fdov8ysdf</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
         </is>
       </c>
     </row>

</xml_diff>